<commit_message>
Added script & outputs to parse EC --> dbCAN outputs
</commit_message>
<xml_diff>
--- a/dbcan/MucinDegTable.xlsx
+++ b/dbcan/MucinDegTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ecf4928fe261446/Documents/GitHub/OG_MetaG/dbcan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3940" documentId="8_{823AC7C7-7085-4180-B3B6-259E9669237A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1E74124F-AECF-4483-90E5-D42934FD2153}"/>
+  <xr:revisionPtr revIDLastSave="3952" documentId="8_{823AC7C7-7085-4180-B3B6-259E9669237A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C9BA26C0-5C03-40AF-A82C-68B166F3E8BE}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{E12190B5-FBFA-48B1-9D43-6098B5871443}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{E12190B5-FBFA-48B1-9D43-6098B5871443}"/>
   </bookViews>
   <sheets>
     <sheet name="Final List" sheetId="6" r:id="rId1"/>
@@ -11427,8 +11427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF3EB00C-3366-4A7B-B49C-AC9EB5EA56B4}">
   <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="G49" sqref="A26:G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>